<commit_message>
after extent, jenkins build etc...
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rakesh\Personal\Courses\Eclipse workspace\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC34B13-CF38-486B-AC09-C30DA64F3F52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF7E038-0B38-467A-8A21-5278527D270E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{0210A7D5-3DCD-48D8-99C1-7606ED86D494}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0210A7D5-3DCD-48D8-99C1-7606ED86D494}"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t>firstName</t>
   </si>
@@ -67,7 +68,52 @@
     <t>manish kumar</t>
   </si>
   <si>
-    <t>rupee</t>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Account created successfully</t>
+  </si>
+  <si>
+    <t>alertMessage</t>
+  </si>
+  <si>
+    <t>rakesh</t>
+  </si>
+  <si>
+    <t>sudesh</t>
+  </si>
+  <si>
+    <t>naveen</t>
+  </si>
+  <si>
+    <t>rakesh kumar</t>
+  </si>
+  <si>
+    <t>sudesh kumar</t>
+  </si>
+  <si>
+    <t>naveen kumar</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>runMode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -418,11 +464,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235D9A1B-0547-43C4-B646-45DB105B59E5}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D30C7FC-EE48-4261-A4FC-F1203C44240B}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +526,7 @@
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,8 +539,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -456,6 +555,60 @@
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -463,33 +616,88 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB937027-44DB-4724-BF9A-02FB38205229}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>